<commit_message>
Updated Registration with few more TC
</commit_message>
<xml_diff>
--- a/qa/Registration-mobAPP.xlsx
+++ b/qa/Registration-mobAPP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
   <si>
     <t>Project Name</t>
   </si>
@@ -72,12 +72,6 @@
     <t>R-003</t>
   </si>
   <si>
-    <t>Registration with all details.</t>
-  </si>
-  <si>
-    <t>Registeration-&gt;All text fields are manadatory.</t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter all or any of the field as null. .
 3. Run TC.</t>
@@ -206,9 +200,6 @@
     <t>R-013</t>
   </si>
   <si>
-    <t xml:space="preserve">Registeration-&gt;mobile number with alphacharacters </t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter mobile with alphacharacters. 
 3. Run TC.</t>
@@ -221,17 +212,11 @@
     <t>R-014</t>
   </si>
   <si>
-    <t>Registeration-&gt;mobile number with special characters</t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter mobile with specialcharacters. 
 3. Run TC.</t>
   </si>
   <si>
-    <t>Registeration-&gt;mobile number with alphanumerics</t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter mobile with alphanumerics. 
 3. Run TC.</t>
@@ -246,9 +231,6 @@
     <t>1. GoTo Registration TC.
 2. Enter invalid email.
 3. Run TC.</t>
-  </si>
-  <si>
-    <t>Registeration-&gt;invalid Email as junk value ("vdhjfhkjfbhjgh")</t>
   </si>
   <si>
     <t>Schema Error,
@@ -258,9 +240,6 @@
     <t>R-017</t>
   </si>
   <si>
-    <t xml:space="preserve">Registeration-&gt; Age with alphacharacters </t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter Age with alphacharacters. 
 3. Run TC.</t>
@@ -270,17 +249,11 @@
 "Age should be integer"</t>
   </si>
   <si>
-    <t xml:space="preserve">Registeration-&gt; Age with alphanumerics </t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter Age with alphanumerics. 
 3. Run TC.</t>
   </si>
   <si>
-    <t xml:space="preserve">Registeration-&gt; Age with specialcharacters </t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter Age with specialcharacters. 
 3. Run TC.</t>
@@ -292,15 +265,6 @@
     <t>R-019</t>
   </si>
   <si>
-    <t>Registeration-&gt;Username which already exists.</t>
-  </si>
-  <si>
-    <t>Registeration-&gt;mobile number which already exists.</t>
-  </si>
-  <si>
-    <t>Registeration-&gt;Email which already registered or exists.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Registration-&gt; invalid Password     </t>
   </si>
   <si>
@@ -316,6 +280,170 @@
     <t>1. GoTo Registration TC.
 2. Enter password &amp; all details.
 3. Run TC.</t>
+  </si>
+  <si>
+    <t>R-020</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing username field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"username should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>R-021</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing password field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"password should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>R-022</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing email field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"email should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>R-023</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing mobile field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"mobile should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>R-024</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing firstname field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"firstname should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing lastname field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"lastname should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing age field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"age should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>R-025</t>
+  </si>
+  <si>
+    <t>R-026</t>
+  </si>
+  <si>
+    <t>R-027</t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. missing gender field.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message,
+"gender should be mandatory"
+</t>
+  </si>
+  <si>
+    <t>Registration by entering all details.</t>
+  </si>
+  <si>
+    <t>Registration-&gt;Username which already exists.</t>
+  </si>
+  <si>
+    <t>Registration-&gt;mobile number which already exists.</t>
+  </si>
+  <si>
+    <t>Registration-&gt;Email which already registered or exists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration-&gt;mobile number with alphacharacters </t>
+  </si>
+  <si>
+    <t>Registration-&gt;mobile number with special characters</t>
+  </si>
+  <si>
+    <t>Registration-&gt;mobile number with alphanumerics</t>
+  </si>
+  <si>
+    <t>Registration-&gt;invalid Email as junk value ("vdhjfhkjfbhjgh")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration-&gt; Age with alphacharacters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration-&gt; Age with alphanumerics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration-&gt; Age with specialcharacters </t>
+  </si>
+  <si>
+    <t>Registration-&gt;username field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;password field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;email field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;mobile field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;firstname field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;lastname field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;Age field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;gender field is missing</t>
+  </si>
+  <si>
+    <t>Registration-&gt;missing value for any or all of the field</t>
   </si>
 </sst>
 </file>
@@ -797,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -870,13 +998,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
@@ -884,13 +1012,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
@@ -898,7 +1026,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>11</v>
@@ -909,227 +1037,345 @@
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="71.25">
       <c r="A12" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="85.5">
       <c r="A13" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="85.5">
       <c r="A14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="85.5">
       <c r="A15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="85.5">
       <c r="A16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
       <c r="A23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="B25" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A26" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A27" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A28" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A29" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="10" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="10" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>